<commit_message>
Final DataFile (Stories sprint1)
</commit_message>
<xml_diff>
--- a/hexaboards/DataFileScripts.xlsx
+++ b/hexaboards/DataFileScripts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="163">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -39,7 +39,7 @@
     <t xml:space="preserve">Ivonne</t>
   </si>
   <si>
-    <t xml:space="preserve">Ivonne1-</t>
+    <t xml:space="preserve">Ivonne-1</t>
   </si>
   <si>
     <t xml:space="preserve">holis</t>
@@ -397,9 +397,6 @@
   </si>
   <si>
     <t xml:space="preserve">Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ivonne-1</t>
   </si>
   <si>
     <t xml:space="preserve">Tests Views</t>
@@ -900,11 +897,11 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.42"/>
@@ -993,11 +990,11 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.89453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.9140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.97"/>
@@ -1615,7 +1612,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.89453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.9140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
   </cols>
@@ -1678,11 +1675,11 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.89453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.9140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.57"/>
   </cols>
@@ -1820,7 +1817,7 @@
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.89453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.9140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -1953,11 +1950,11 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.8"/>
   </cols>
@@ -2063,11 +2060,11 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.02"/>
@@ -2106,19 +2103,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="D2" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="E2" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="33" t="s">
-        <v>126</v>
-      </c>
       <c r="F2" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
@@ -2128,22 +2125,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C3" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="F3" s="33" t="s">
+      <c r="G3" s="33" t="s">
         <v>128</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>129</v>
       </c>
       <c r="H3" s="33" t="s">
         <v>2</v>
@@ -2154,19 +2151,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C4" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="E4" s="33" t="s">
+      <c r="F4" s="33" t="s">
         <v>131</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>132</v>
       </c>
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
@@ -2176,22 +2173,22 @@
         <v>2</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C5" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>134</v>
-      </c>
       <c r="E5" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F5" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="33" t="s">
         <v>128</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>129</v>
       </c>
       <c r="H5" s="33" t="s">
         <v>2</v>
@@ -2202,19 +2199,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D6" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="33" t="s">
-        <v>126</v>
-      </c>
       <c r="F6" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
@@ -2224,17 +2221,17 @@
         <v>2</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
@@ -2244,19 +2241,19 @@
         <v>2</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C8" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>138</v>
-      </c>
       <c r="E8" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
@@ -2266,19 +2263,19 @@
         <v>2</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C9" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="E9" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="E9" s="33" t="s">
-        <v>141</v>
-      </c>
       <c r="F9" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
@@ -2288,14 +2285,14 @@
         <v>2</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F10" s="35" t="n">
         <v>44085</v>
@@ -2308,19 +2305,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C11" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="33" t="s">
         <v>144</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>145</v>
       </c>
       <c r="E11" s="36" t="n">
         <v>43737</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
@@ -2330,16 +2327,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C12" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="33" t="s">
-        <v>147</v>
-      </c>
       <c r="E12" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="34"/>
@@ -2350,16 +2347,16 @@
         <v>2</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C13" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>149</v>
-      </c>
       <c r="E13" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
@@ -2370,13 +2367,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C14" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="33" t="s">
         <v>150</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>151</v>
       </c>
       <c r="E14" s="34"/>
       <c r="F14" s="34"/>
@@ -2388,19 +2385,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C15" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" s="33" t="s">
         <v>152</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>153</v>
       </c>
       <c r="E15" s="35" t="n">
         <v>43686</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
@@ -2410,7 +2407,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C16" s="34"/>
       <c r="D16" s="34"/>
@@ -2424,7 +2421,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
@@ -2438,19 +2435,19 @@
         <v>2</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C18" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="D18" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="E18" s="33" t="s">
+      <c r="F18" s="33" t="s">
         <v>156</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>157</v>
       </c>
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
@@ -2460,20 +2457,20 @@
         <v>2</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C19" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="E19" s="33" t="s">
         <v>159</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>160</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H19" s="33" t="s">
         <v>2</v>
@@ -2498,10 +2495,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.86"/>
@@ -2557,11 +2554,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.26"/>
@@ -2588,20 +2585,20 @@
         <v>10</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="D2" s="37" t="s">
         <v>162</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>163</v>
       </c>
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="554@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="ivon554@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>